<commit_message>
Auskommentieren der export Funktion
</commit_message>
<xml_diff>
--- a/Gebaeudedaten.xlsx
+++ b/Gebaeudedaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\PycharmProjects\TeaserTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FD475E-1A7B-479F-B02A-CDFD51C65461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B4B959-F7AF-49B8-B92F-79E320F12B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{080B8E1F-70F6-4242-9D79-9D2FF512E4FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>WG Roermonder</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Flaeche (net_leased_area)</t>
+  </si>
+  <si>
+    <t>Griessgram</t>
   </si>
 </sst>
 </file>
@@ -161,11 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -480,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B18ADF-D660-4FA9-B5C6-6C65AB25CFE4}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,53 +492,53 @@
     <col min="5" max="5" width="15.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -685,6 +686,29 @@
       </c>
       <c r="O5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>1998</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.76</v>
+      </c>
+      <c r="F6">
+        <v>5000</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
advanced_buildings hinzugefuegt, kleiner Aenderungen in main.py
</commit_message>
<xml_diff>
--- a/Gebaeudedaten.xlsx
+++ b/Gebaeudedaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\PycharmProjects\TeaserTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B4B959-F7AF-49B8-B92F-79E320F12B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0A96F5-F6E7-4016-8013-D5B7804FC62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{080B8E1F-70F6-4242-9D79-9D2FF512E4FB}"/>
   </bookViews>
@@ -83,30 +83,18 @@
     <t>streetname</t>
   </si>
   <si>
-    <t>Roermonder Str. 79</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
     <t>Aachen</t>
   </si>
   <si>
-    <t>Bachstraße 4</t>
-  </si>
-  <si>
     <t>Freiburg</t>
   </si>
   <si>
-    <t>Muehlenstraße 21f</t>
-  </si>
-  <si>
     <t>Duisburg</t>
   </si>
   <si>
-    <t>Vaalser Str. 226</t>
-  </si>
-  <si>
     <t>plz</t>
   </si>
   <si>
@@ -129,6 +117,18 @@
   </si>
   <si>
     <t>Griessgram</t>
+  </si>
+  <si>
+    <t>RoermonderStr.79</t>
+  </si>
+  <si>
+    <t>Bachstraße4</t>
+  </si>
+  <si>
+    <t>Muehlenstraße21f</t>
+  </si>
+  <si>
+    <t>VaalserStr.226</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B18ADF-D660-4FA9-B5C6-6C65AB25CFE4}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,22 +494,22 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -536,10 +536,10 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -574,10 +574,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -612,10 +612,10 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -650,10 +650,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -682,15 +682,15 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>1998</v>

</xml_diff>